<commit_message>
add export from sql command
</commit_message>
<xml_diff>
--- a/data/system/address/v1.xlsx
+++ b/data/system/address/v1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022C18AB-DAF8-E04A-9680-164844258F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1461638-5142-7448-AFC1-2FD68DCA3895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="2620" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4730,12 +4730,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fix a issue caused by : in []
</commit_message>
<xml_diff>
--- a/data/system/address/v1.xlsx
+++ b/data/system/address/v1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696BC5E7-210D-ED43-82FD-2F82BBC7A09D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5F07C3-BED7-2C4B-824F-C454ED8F2C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="2620" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4447,9 +4447,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -4728,7 +4731,7 @@
   <dimension ref="A1:E373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4767,7 +4770,7 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new features for 1.1
</commit_message>
<xml_diff>
--- a/data/system/address/v1.xlsx
+++ b/data/system/address/v1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18158B4A-1497-424E-B3A9-8D4E0FAD08E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B048D6C-FD4C-3847-9844-B56CCC216AEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="2620" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4745,7 +4745,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H373"/>
+  <dimension ref="A1:F373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -4757,7 +4757,7 @@
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -4912,11 +4912,8 @@
       <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -4933,7 +4930,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -4950,7 +4947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -4967,7 +4964,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -4984,7 +4981,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -5001,7 +4998,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -5018,7 +5015,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>